<commit_message>
Added acceleromter, some notes
</commit_message>
<xml_diff>
--- a/PartsList.xlsx
+++ b/PartsList.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffthompson/Documents/PhysicalComputing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B241400-23D5-3446-81F2-A0D2F4AE93AE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4C83FB5D-E30A-3444-977F-3D7A4C8C7D02}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9000" yWindow="460" windowWidth="29400" windowHeight="21140" xr2:uid="{B16D493A-A945-0C40-AA37-D72AEF9A0E93}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="92">
   <si>
     <t>BILL OF MATERIALS</t>
   </si>
@@ -108,9 +108,6 @@
     <t>https://www.sparkfun.com/products/8022</t>
   </si>
   <si>
-    <t>Hookup wire (any color ok)</t>
-  </si>
-  <si>
     <t>OPTIONAL</t>
   </si>
   <si>
@@ -289,6 +286,21 @@
   </si>
   <si>
     <t>(Amazon link for hookup wire is more  $$ but comes with 6 spools, so you could share)</t>
+  </si>
+  <si>
+    <t>3-axis accelerometer</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/13926</t>
+  </si>
+  <si>
+    <t>RGB light sensor</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/12829</t>
+  </si>
+  <si>
+    <t>Hookup wire (stranded is best, any color ok)</t>
   </si>
 </sst>
 </file>
@@ -688,10 +700,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E11B348E-E77B-E746-8713-31BB8A7C73ED}">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -728,10 +740,10 @@
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -752,7 +764,7 @@
         <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -773,7 +785,7 @@
         <v>16</v>
       </c>
       <c r="F6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -805,15 +817,15 @@
         <v>5.95</v>
       </c>
       <c r="E8" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B9" s="4">
         <v>1.95</v>
@@ -826,10 +838,10 @@
         <v>3.9</v>
       </c>
       <c r="E9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F9" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -850,7 +862,7 @@
         <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -871,7 +883,7 @@
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -892,7 +904,7 @@
         <v>25</v>
       </c>
       <c r="F12" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -913,12 +925,12 @@
         <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="B14" s="4">
         <v>2.5</v>
@@ -934,12 +946,12 @@
         <v>26</v>
       </c>
       <c r="F14" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="F15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="21" x14ac:dyDescent="0.25">
@@ -966,7 +978,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B18" s="4">
         <v>1.5</v>
@@ -979,7 +991,7 @@
         <v>4.5</v>
       </c>
       <c r="E18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -997,7 +1009,7 @@
         <v>1.5</v>
       </c>
       <c r="E19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
@@ -1015,12 +1027,12 @@
         <v>3.9</v>
       </c>
       <c r="E20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B21" s="4">
         <v>10.95</v>
@@ -1033,12 +1045,12 @@
         <v>10.95</v>
       </c>
       <c r="E21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B22" s="4">
         <v>1.5</v>
@@ -1051,7 +1063,7 @@
         <v>1.5</v>
       </c>
       <c r="E22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -1069,12 +1081,12 @@
         <v>1.95</v>
       </c>
       <c r="E23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
@@ -1096,7 +1108,7 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B27" s="4">
         <v>0.95</v>
@@ -1105,16 +1117,16 @@
         <v>1</v>
       </c>
       <c r="D27" s="4">
-        <f t="shared" ref="D27:D31" si="2">C27*B27</f>
+        <f t="shared" ref="D27:D33" si="2">C27*B27</f>
         <v>0.95</v>
       </c>
       <c r="E27" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B28" s="4">
         <v>3.95</v>
@@ -1127,12 +1139,12 @@
         <v>3.95</v>
       </c>
       <c r="E28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B29" s="4">
         <v>14.95</v>
@@ -1145,12 +1157,12 @@
         <v>14.95</v>
       </c>
       <c r="E29" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B30" s="4">
         <v>1.95</v>
@@ -1163,12 +1175,12 @@
         <v>1.95</v>
       </c>
       <c r="E30" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B31" s="4">
         <v>2.95</v>
@@ -1181,219 +1193,219 @@
         <v>2.95</v>
       </c>
       <c r="E31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A34" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B32" s="4">
+        <v>10.49</v>
+      </c>
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" s="4">
+        <f t="shared" si="2"/>
+        <v>10.49</v>
+      </c>
+      <c r="E32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>89</v>
+      </c>
+      <c r="B33" s="4">
+        <v>7.95</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33" s="4">
+        <f t="shared" si="2"/>
+        <v>7.95</v>
+      </c>
+      <c r="E33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="21" x14ac:dyDescent="0.25">
+      <c r="A36" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A35" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D35" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="B38" s="4">
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="C38">
+        <v>1</v>
+      </c>
+      <c r="D38" s="4">
+        <f t="shared" ref="D38:D48" si="3">C38*B38</f>
+        <v>9.9499999999999993</v>
+      </c>
+      <c r="E38" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
         <v>29</v>
       </c>
-      <c r="B36" s="4">
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" s="4">
-        <f t="shared" ref="D36:D46" si="3">C36*B36</f>
-        <v>9.9499999999999993</v>
-      </c>
-      <c r="E36" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>30</v>
-      </c>
-      <c r="B37" s="4">
+      <c r="B39" s="4">
         <v>16.95</v>
       </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37" s="4">
+      <c r="C39">
+        <v>1</v>
+      </c>
+      <c r="D39" s="4">
         <f t="shared" si="3"/>
         <v>16.95</v>
       </c>
-      <c r="E37" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>33</v>
-      </c>
-      <c r="B38" s="4">
+      <c r="E39" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>32</v>
+      </c>
+      <c r="B40" s="4">
         <v>1.95</v>
       </c>
-      <c r="C38">
-        <v>1</v>
-      </c>
-      <c r="D38" s="4">
+      <c r="C40">
+        <v>1</v>
+      </c>
+      <c r="D40" s="4">
         <f t="shared" si="3"/>
         <v>1.95</v>
       </c>
-      <c r="E38" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="4">
+      <c r="E40" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="4">
         <v>7.95</v>
       </c>
-      <c r="C39">
-        <v>1</v>
-      </c>
-      <c r="D39" s="4">
+      <c r="C41">
+        <v>1</v>
+      </c>
+      <c r="D41" s="4">
         <f t="shared" si="3"/>
         <v>7.95</v>
       </c>
-      <c r="E39" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>39</v>
-      </c>
-      <c r="B40" s="4">
+      <c r="E41" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" s="4">
         <v>5.95</v>
       </c>
-      <c r="C40">
-        <v>1</v>
-      </c>
-      <c r="D40" s="4">
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" s="4">
         <f t="shared" si="3"/>
         <v>5.95</v>
       </c>
-      <c r="E40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>62</v>
-      </c>
-      <c r="B41" s="4">
+      <c r="E42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>61</v>
+      </c>
+      <c r="B43" s="4">
         <v>9.9499999999999993</v>
       </c>
-      <c r="C41">
-        <v>1</v>
-      </c>
-      <c r="D41" s="4">
+      <c r="C43">
+        <v>1</v>
+      </c>
+      <c r="D43" s="4">
         <f t="shared" si="3"/>
         <v>9.9499999999999993</v>
       </c>
-      <c r="E41" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>63</v>
-      </c>
-      <c r="B42" s="4">
+      <c r="E43" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>62</v>
+      </c>
+      <c r="B44" s="4">
         <v>7.95</v>
       </c>
-      <c r="C42">
-        <v>1</v>
-      </c>
-      <c r="D42" s="4">
+      <c r="C44">
+        <v>1</v>
+      </c>
+      <c r="D44" s="4">
         <f t="shared" si="3"/>
         <v>7.95</v>
       </c>
-      <c r="E42" t="s">
+      <c r="E44" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>68</v>
-      </c>
-      <c r="B43" s="4">
+      <c r="B45" s="4">
         <v>2.95</v>
       </c>
-      <c r="C43">
-        <v>1</v>
-      </c>
-      <c r="D43" s="4">
+      <c r="C45">
+        <v>1</v>
+      </c>
+      <c r="D45" s="4">
         <f t="shared" si="3"/>
         <v>2.95</v>
       </c>
-      <c r="E43" t="s">
+      <c r="E45" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>69</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>70</v>
-      </c>
-      <c r="B44" s="4">
-        <v>4.95</v>
-      </c>
-      <c r="C44">
-        <v>1</v>
-      </c>
-      <c r="D44" s="4">
-        <f t="shared" si="3"/>
-        <v>4.95</v>
-      </c>
-      <c r="E44" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>64</v>
-      </c>
-      <c r="B45" s="4">
-        <v>23.5</v>
-      </c>
-      <c r="C45">
-        <v>1</v>
-      </c>
-      <c r="D45" s="4">
-        <f t="shared" si="3"/>
-        <v>23.5</v>
-      </c>
-      <c r="E45" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" ht="20" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>65</v>
       </c>
       <c r="B46" s="4">
         <v>4.95</v>
@@ -1405,21 +1417,57 @@
         <f t="shared" si="3"/>
         <v>4.95</v>
       </c>
-      <c r="E46" s="6" t="s">
-        <v>73</v>
+      <c r="E46" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47" s="4">
+        <v>23.5</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47" s="4">
+        <f t="shared" si="3"/>
+        <v>23.5</v>
+      </c>
+      <c r="E47" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" ht="20" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>64</v>
+      </c>
+      <c r="B48" s="4">
+        <v>4.95</v>
+      </c>
+      <c r="C48">
+        <v>1</v>
+      </c>
+      <c r="D48" s="4">
+        <f t="shared" si="3"/>
+        <v>4.95</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>73</v>
+      </c>
+      <c r="B49" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="C47">
-        <v>1</v>
-      </c>
-      <c r="D47" t="s">
+      <c r="C49">
+        <v>1</v>
+      </c>
+      <c r="D49" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>